<commit_message>
submodulo do projeto adicionado
</commit_message>
<xml_diff>
--- a/Gerenciamento de Projeto/Checklist Verificacao de Projeto Grupo 7.xlsx
+++ b/Gerenciamento de Projeto/Checklist Verificacao de Projeto Grupo 7.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{EDCD60E5-50E4-7741-99B7-80E0A3A03BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B580EF4A-97C1-EE4A-8771-08881C581CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicadores" sheetId="6" r:id="rId1"/>
@@ -628,7 +628,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="125">
   <si>
     <t>Ambiente</t>
   </si>
@@ -1000,6 +1000,9 @@
   </si>
   <si>
     <t>Sim</t>
+  </si>
+  <si>
+    <t>CheckList de Verificação de Projeto - FEITO PELO GRUPO 6</t>
   </si>
 </sst>
 </file>
@@ -2062,8 +2065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -2078,7 +2081,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="19.5" customHeight="1">
       <c r="A1" s="31" t="s">
-        <v>16</v>
+        <v>124</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
@@ -4065,17 +4068,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:F3"/>
     <mergeCell ref="A5:A16"/>
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A22:A28"/>
     <mergeCell ref="A37:A43"/>
     <mergeCell ref="A44:A51"/>
     <mergeCell ref="A29:A36"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:F3"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D10:D12 D14 D8 D16:D49" xr:uid="{00000000-0002-0000-0300-000000000000}">
@@ -4732,11 +4735,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="A35:A42"/>
-    <mergeCell ref="A43:A50"/>
-    <mergeCell ref="A19:A24"/>
-    <mergeCell ref="A29:A34"/>
     <mergeCell ref="A5:A16"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A1:F1"/>
@@ -4744,6 +4742,11 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="A43:A50"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="A29:A34"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D10:D12 D14 D8 D16:D48" xr:uid="{00000000-0002-0000-0400-000000000000}">

</xml_diff>